<commit_message>
validate fullname contain digit
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Bang tot nghiep loi.xlsx
+++ b/eCert/Uploads/Bang tot nghiep loi.xlsx
@@ -74,9 +74,6 @@
     <t>HE130603</t>
   </si>
   <si>
-    <t>Hoang Viet Bach</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>3a/3/2021</t>
+  </si>
+  <si>
+    <t>Hoang Viet Bach0</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,31 +499,31 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1">
         <v>36479</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -531,28 +531,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>36465</v>
       </c>
       <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
       </c>
       <c r="J3" s="1">
         <v>44258</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>23</v>
-      </c>
-      <c r="N3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test import certificate of Admin
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Bang tot nghiep loi.xlsx
+++ b/eCert/Uploads/Bang tot nghiep loi.xlsx
@@ -74,6 +74,9 @@
     <t>HE130603</t>
   </si>
   <si>
+    <t>Hoang Viet Bach</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -102,9 +105,6 @@
   </si>
   <si>
     <t>3a/3/2021</t>
-  </si>
-  <si>
-    <t>Hoang Viet Bach0</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,31 +499,31 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>36479</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -531,28 +531,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
         <v>36465</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1">
         <v>44258</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test import diploma -Admin
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Bang tot nghiep loi.xlsx
+++ b/eCert/Uploads/Bang tot nghiep loi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BachHV\Desktop\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169899EA-799A-42C2-A3B8-C7AD1996067E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="600" yWindow="2670" windowWidth="27990" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -105,12 +106,39 @@
   </si>
   <si>
     <t>3a/3/2021</t>
+  </si>
+  <si>
+    <t>HE130604</t>
+  </si>
+  <si>
+    <t>Pham Thanh Ha</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>QD@@</t>
+  </si>
+  <si>
+    <t>$$</t>
+  </si>
+  <si>
+    <t>ĐH 23232</t>
+  </si>
+  <si>
+    <t>ES2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,11 +450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +561,9 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
       <c r="D3" s="1">
         <v>36465</v>
       </c>
@@ -553,6 +584,44 @@
       </c>
       <c r="N3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="1">
+        <v>54850</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>